<commit_message>
wireframes - ui simple
</commit_message>
<xml_diff>
--- a/documentation/risklist.xlsx
+++ b/documentation/risklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD045FBF-56F6-4CC5-BD4A-BD13AD4278D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB10A1CC-4755-438B-B41D-82A5D2088594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,9 +64,6 @@
     <t>Mitigační akce</t>
   </si>
   <si>
-    <t>Popis riziko</t>
-  </si>
-  <si>
     <t>Pravděpodobnost</t>
   </si>
   <si>
@@ -98,6 +95,9 @@
   </si>
   <si>
     <t>Průběžné konzultace (např. jednou týdně, jednou za dva týdny) s demonstrací pokroku a zpětnou vazbou od zákazníka.</t>
+  </si>
+  <si>
+    <t>Popis rizika</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,10 +516,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -528,7 +528,7 @@
         <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -536,13 +536,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>1</v>
@@ -559,10 +559,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>2</v>
@@ -579,10 +579,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>11</v>
@@ -599,10 +599,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>5</v>
@@ -619,13 +619,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="10">
         <v>1</v>
@@ -639,13 +639,13 @@
         <v>12</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="10">
         <v>1</v>
@@ -656,16 +656,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="10">
         <v>1</v>
@@ -676,13 +676,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>10</v>
@@ -699,10 +699,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>9</v>

</xml_diff>